<commit_message>
Adding spring boot crud application and API tests for it
</commit_message>
<xml_diff>
--- a/resources/Test_Cases.xlsx
+++ b/resources/Test_Cases.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aspen User\eclipse-workspace\JiveTestv2\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aspen User\git\AutoTestsProject\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Header" sheetId="11" r:id="rId1"/>
     <sheet name="Parameters" sheetId="13" r:id="rId2"/>
-    <sheet name="getByEmail" sheetId="14" r:id="rId3"/>
+    <sheet name="products" sheetId="14" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Content-Type</t>
   </si>
@@ -58,7 +58,25 @@
     <t>GLOBAL_QUOTE</t>
   </si>
   <si>
-    <t>{}</t>
+    <t>{
+ "name":"mouse",
+ "description":"mouse_description",
+ "price":10.14
+}</t>
+  </si>
+  <si>
+    <t>{
+ "name":"keyBoard",
+ "description":"104 button keyboard",
+ "price":20.33
+}</t>
+  </si>
+  <si>
+    <t>{
+ "name":"laptop",
+ "description":"laptop_description",
+ "price":999.99
+}</t>
   </si>
 </sst>
 </file>
@@ -113,11 +131,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -475,17 +496,30 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="33.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding a SOAP WebSerivce to the Spring boot and SAAJ tests
</commit_message>
<xml_diff>
--- a/resources/Test_Cases.xlsx
+++ b/resources/Test_Cases.xlsx
@@ -3,20 +3,17 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aspen User\git\AutoTestsProject\resources\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15945" windowHeight="3240" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Header" sheetId="11" r:id="rId1"/>
     <sheet name="Parameters" sheetId="13" r:id="rId2"/>
     <sheet name="products" sheetId="14" r:id="rId3"/>
+    <sheet name="soapMimeHeaders" sheetId="17" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1:P8"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t>Content-Type</t>
   </si>
@@ -78,12 +75,21 @@
  "price":999.99
 }</t>
   </si>
+  <si>
+    <t>application/xml</t>
+  </si>
+  <si>
+    <t>SOAPAction</t>
+  </si>
+  <si>
+    <t>http://application.com/soap/products/addProductRequest</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -110,6 +116,14 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -128,10 +142,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -139,8 +154,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -421,7 +438,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -525,4 +542,38 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>